<commit_message>
Updated the burndow chart file
Corrected an error in the burndown chart file.
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 2/Sprint 2 Burndown Chart.xlsx
+++ b/Project/Phase 1/Sprint 2/Sprint 2 Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Downloads\EstudoDT\3ºano\ES\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B7D979-46F9-48B7-B31E-825A7FE6BE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B186A1F8-FA45-4DD0-8528-1BC9D6E32BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A5DD4D7C-BA4F-4A0D-9493-D2A15D6A6BE5}"/>
   </bookViews>
@@ -369,22 +369,22 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>18.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>17.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,7 +1495,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="1">
-        <v>18.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1">
-        <v>18</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>17.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>10</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>